<commit_message>
lots of stuff - eliminate more underscore prefixed arguments - update spreadsheet - small cleanup in caching server - correct block hash stuff to get hash from previous block - separate scaling out in QuadraticBondingCurve - test events for deep gems contract - update numbers in bonding curve test
</commit_message>
<xml_diff>
--- a/solidity/deep-gems-numbers.xlsx
+++ b/solidity/deep-gems-numbers.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jehan/projects/deep-gems/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jehan/projects/deepgems/solidity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4387932-0512-FE49-8486-668E889E83B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4AD799-81D8-3C43-A4DC-45AADF8CB493}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{71828AD9-EA99-1C4A-A456-5EB5551B9F92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>unscaled ..1</t>
   </si>
@@ -39,25 +39,31 @@
     <t>Dollar market cap</t>
   </si>
   <si>
-    <t>Dollar cost to mint one</t>
-  </si>
-  <si>
     <t>Ether price</t>
   </si>
   <si>
     <t>Scaling factor</t>
   </si>
   <si>
-    <t>Gem number</t>
-  </si>
-  <si>
-    <t>Gem number:</t>
-  </si>
-  <si>
     <t>unscaled ..+1</t>
   </si>
   <si>
     <t>unscaled ..+1 - ..1</t>
+  </si>
+  <si>
+    <t>Token number:</t>
+  </si>
+  <si>
+    <t>Token number</t>
+  </si>
+  <si>
+    <t>Dollar cost to mint token</t>
+  </si>
+  <si>
+    <t>Dollar cost to mint one gem with 100 psi</t>
+  </si>
+  <si>
+    <t>Gem number (approx)</t>
   </si>
 </sst>
 </file>
@@ -66,8 +72,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.000000000000000000_);_(* \(#,##0.000000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -120,15 +126,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -444,56 +451,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3F3CE4-B0B2-B443-B4D2-87B823B17513}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="26.83203125" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="38.5" customWidth="1"/>
+    <col min="8" max="8" width="35.1640625" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" customWidth="1"/>
+    <col min="11" max="11" width="34.6640625" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="5">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1000000000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5">
         <v>1700</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
@@ -505,112 +512,134 @@
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
       </c>
       <c r="L4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2">
         <f t="shared" ref="C5:C6" si="0">(A5^3 / 3)</f>
-        <v>0.33333333333333331</v>
+        <v>333333.33333333331</v>
       </c>
       <c r="D5" s="3">
         <f>((A5+1)^3 / 3)</f>
-        <v>2.6666666666666665</v>
+        <v>343433.66666666669</v>
       </c>
       <c r="E5" s="3">
         <f>D5-C5</f>
-        <v>2.333333333333333</v>
-      </c>
-      <c r="G5" s="3">
+        <v>10100.333333333372</v>
+      </c>
+      <c r="G5" s="8">
         <f t="shared" ref="G5:G6" si="1">C5/$B$1</f>
         <v>3.333333333333333E-7</v>
       </c>
-      <c r="H5" s="7">
-        <f t="shared" ref="H5:H6" si="2">E5/$B$1</f>
-        <v>2.3333333333333332E-6</v>
+      <c r="H5" s="8">
+        <f>E5/$B$1</f>
+        <v>1.0100333333333372E-8</v>
       </c>
       <c r="I5" s="3">
-        <f t="shared" ref="I5:I6" si="3">G5*$B$2</f>
+        <f t="shared" ref="I5:I6" si="2">G5*$B$2</f>
         <v>5.666666666666666E-4</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" ref="J5:J6" si="4">H5*$B$2</f>
-        <v>3.9666666666666661E-3</v>
+        <f t="shared" ref="J5:J6" si="3">H5*$B$2</f>
+        <v>1.7170566666666732E-5</v>
+      </c>
+      <c r="K5" s="3">
+        <f>J5*100</f>
+        <v>1.7170566666666733E-3</v>
       </c>
       <c r="L5" s="6">
         <f>A5</f>
+        <v>100</v>
+      </c>
+      <c r="M5" s="7">
+        <f>L5/100</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>333.33333333333331</v>
+        <v>333333333.33333331</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" ref="D6:D13" si="5">((A6+1)^3 / 3)</f>
-        <v>443.66666666666669</v>
+        <f t="shared" ref="D6:D13" si="4">((A6+1)^3 / 3)</f>
+        <v>334334333.66666669</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" ref="E6:E13" si="6">D6-C6</f>
-        <v>110.33333333333337</v>
-      </c>
-      <c r="G6" s="3">
+        <f t="shared" ref="E6:E13" si="5">D6-C6</f>
+        <v>1001000.3333333731</v>
+      </c>
+      <c r="G6" s="8">
         <f t="shared" si="1"/>
         <v>3.3333333333333332E-4</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="8">
+        <f t="shared" ref="H5:H6" si="6">E6/$B$1</f>
+        <v>1.001000333333373E-6</v>
+      </c>
+      <c r="I6" s="3">
         <f t="shared" si="2"/>
-        <v>1.1033333333333338E-4</v>
-      </c>
-      <c r="I6" s="3">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="J6" s="3">
         <f t="shared" si="3"/>
-        <v>0.56666666666666665</v>
-      </c>
-      <c r="J6" s="3">
-        <f t="shared" si="4"/>
-        <v>0.18756666666666674</v>
+        <v>1.7017005666667342E-3</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" ref="K6:K13" si="7">J6*100</f>
+        <v>0.17017005666667342</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" ref="L6:L13" si="7">A6</f>
+        <f t="shared" ref="L6:L13" si="8">A6</f>
+        <v>1000</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" ref="M6:M13" si="9">L6/100</f>
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2">
         <f>(A7^3 / 3)</f>
-        <v>333333.33333333331</v>
+        <v>333333333333.33331</v>
       </c>
       <c r="D7" s="3">
+        <f t="shared" si="4"/>
+        <v>333433343333.66669</v>
+      </c>
+      <c r="E7" s="3">
         <f t="shared" si="5"/>
-        <v>343433.66666666669</v>
-      </c>
-      <c r="E7" s="3">
-        <f t="shared" si="6"/>
-        <v>10100.333333333372</v>
-      </c>
-      <c r="G7" s="3">
+        <v>100010000.33337402</v>
+      </c>
+      <c r="G7" s="8">
         <f>C7/$B$1</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="8">
         <f>E7/$B$1</f>
-        <v>1.0100333333333373E-2</v>
+        <v>1.0001000033337402E-4</v>
       </c>
       <c r="I7" s="3">
         <f>G7*$B$2</f>
@@ -618,238 +647,294 @@
       </c>
       <c r="J7" s="3">
         <f>H7*$B$2</f>
-        <v>17.170566666666733</v>
+        <v>0.17001700056673583</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="7"/>
+        <v>17.001700056673581</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="M7" s="7">
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>200</v>
+        <v>20000</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2">
-        <f t="shared" ref="C8:C13" si="8">(A8^3 / 3)</f>
-        <v>2666666.6666666665</v>
+        <f t="shared" ref="C8:C13" si="10">(A8^3 / 3)</f>
+        <v>2666666666666.6665</v>
       </c>
       <c r="D8" s="3">
+        <f t="shared" si="4"/>
+        <v>2667066686667</v>
+      </c>
+      <c r="E8" s="3">
         <f t="shared" si="5"/>
-        <v>2706867</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="6"/>
-        <v>40200.333333333489</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" ref="G8:G13" si="9">C8/$B$1</f>
+        <v>400020000.33349609</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" ref="G8:G13" si="11">C8/$B$1</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="H8" s="7">
-        <f t="shared" ref="H8:H13" si="10">E8/$B$1</f>
-        <v>4.0200333333333491E-2</v>
+      <c r="H8" s="8">
+        <f t="shared" ref="H8:H13" si="12">E8/$B$1</f>
+        <v>4.000200003334961E-4</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" ref="I8:I13" si="11">G8*$B$2</f>
+        <f t="shared" ref="I8:I13" si="13">G8*$B$2</f>
         <v>4533.333333333333</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" ref="J8:J13" si="12">H8*$B$2</f>
-        <v>68.34056666666693</v>
+        <f t="shared" ref="J8:J13" si="14">H8*$B$2</f>
+        <v>0.68003400056694341</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="7"/>
+        <v>68.003400056694346</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
+        <v>20000</v>
+      </c>
+      <c r="M8" s="7">
+        <f t="shared" si="9"/>
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>300</v>
+        <v>30000</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2">
+        <f t="shared" si="10"/>
+        <v>9000000000000</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="4"/>
+        <v>9000900030000.334</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="5"/>
+        <v>900030000.33398438</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="12"/>
+        <v>9.0003000033398437E-4</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="13"/>
+        <v>15300</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="14"/>
+        <v>1.5300510005677734</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="7"/>
+        <v>153.00510005677734</v>
+      </c>
+      <c r="L9" s="6">
         <f t="shared" si="8"/>
-        <v>9000000</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" si="5"/>
-        <v>9090300.333333334</v>
-      </c>
-      <c r="E9" s="3">
-        <f t="shared" si="6"/>
-        <v>90300.333333333954</v>
-      </c>
-      <c r="G9" s="3">
+        <v>30000</v>
+      </c>
+      <c r="M9" s="7">
         <f t="shared" si="9"/>
-        <v>9</v>
-      </c>
-      <c r="H9" s="7">
-        <f t="shared" si="10"/>
-        <v>9.0300333333333954E-2</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" si="11"/>
-        <v>15300</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="12"/>
-        <v>153.51056666666773</v>
-      </c>
-      <c r="L9" s="6">
-        <f t="shared" si="7"/>
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>2000</v>
+        <v>200000</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2">
+        <f t="shared" si="10"/>
+        <v>2666666666666666.5</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="4"/>
+        <v>2666706666866667</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="5"/>
+        <v>40000200000.5</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="11"/>
+        <v>2666.6666666666665</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="12"/>
+        <v>4.0000200000500002E-2</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="13"/>
+        <v>4533333.333333333</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="14"/>
+        <v>68.000340000850002</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="7"/>
+        <v>6800.0340000850001</v>
+      </c>
+      <c r="L10" s="6">
         <f t="shared" si="8"/>
-        <v>2666666666.6666665</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="5"/>
-        <v>2670668667</v>
-      </c>
-      <c r="E10" s="3">
-        <f t="shared" si="6"/>
-        <v>4002000.3333334923</v>
-      </c>
-      <c r="G10" s="3">
+        <v>200000</v>
+      </c>
+      <c r="M10" s="7">
         <f t="shared" si="9"/>
-        <v>2666.6666666666665</v>
-      </c>
-      <c r="H10" s="7">
-        <f t="shared" si="10"/>
-        <v>4.0020003333334921</v>
-      </c>
-      <c r="I10" s="3">
-        <f t="shared" si="11"/>
-        <v>4533333.333333333</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="12"/>
-        <v>6803.4005666669364</v>
-      </c>
-      <c r="L10" s="6">
-        <f t="shared" si="7"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>9000</v>
+        <v>900000</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2">
+        <f t="shared" si="10"/>
+        <v>2.43E+17</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="4"/>
+        <v>2.430008100009E+17</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="5"/>
+        <v>810000900000</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="11"/>
+        <v>243000</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="12"/>
+        <v>0.81000090000000002</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="13"/>
+        <v>413100000</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="14"/>
+        <v>1377.00153</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="7"/>
+        <v>137700.15299999999</v>
+      </c>
+      <c r="L11" s="6">
         <f t="shared" si="8"/>
-        <v>243000000000</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="5"/>
-        <v>243081009000.33334</v>
-      </c>
-      <c r="E11" s="3">
-        <f t="shared" si="6"/>
-        <v>81009000.333343506</v>
-      </c>
-      <c r="G11" s="3">
+        <v>900000</v>
+      </c>
+      <c r="M11" s="7">
         <f t="shared" si="9"/>
-        <v>243000</v>
-      </c>
-      <c r="H11" s="7">
-        <f t="shared" si="10"/>
-        <v>81.009000333343508</v>
-      </c>
-      <c r="I11" s="3">
-        <f t="shared" si="11"/>
-        <v>413100000</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="12"/>
-        <v>137715.30056668396</v>
-      </c>
-      <c r="L11" s="6">
-        <f t="shared" si="7"/>
         <v>9000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2">
+        <f t="shared" si="10"/>
+        <v>3.3333333333333331E+17</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="4"/>
+        <v>3.3333433333433338E+17</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="5"/>
+        <v>1000001000064</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="11"/>
+        <v>333333.33333333331</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="12"/>
+        <v>1.0000010000640001</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="13"/>
+        <v>566666666.66666663</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="14"/>
+        <v>1700.0017001088002</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="7"/>
+        <v>170000.17001088001</v>
+      </c>
+      <c r="L12" s="6">
         <f t="shared" si="8"/>
-        <v>333333333333.33331</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="5"/>
-        <v>333433343333.66669</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="6"/>
-        <v>100010000.33337402</v>
-      </c>
-      <c r="G12" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="M12" s="7">
         <f t="shared" si="9"/>
-        <v>333333.33333333331</v>
-      </c>
-      <c r="H12" s="7">
-        <f t="shared" si="10"/>
-        <v>100.01000033337402</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" si="11"/>
-        <v>566666666.66666663</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="12"/>
-        <v>170017.00056673583</v>
-      </c>
-      <c r="L12" s="6">
-        <f t="shared" si="7"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>100000</v>
+        <v>10000000</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2">
+        <f t="shared" si="10"/>
+        <v>3.3333333333333331E+20</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="4"/>
+        <v>3.3333343333334332E+20</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="5"/>
+        <v>100000010010624</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="11"/>
+        <v>333333333.33333331</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="12"/>
+        <v>100.000010010624</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="13"/>
+        <v>566666666666.66663</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="14"/>
+        <v>170000.01701806078</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="7"/>
+        <v>17000001.70180608</v>
+      </c>
+      <c r="L13" s="6">
         <f t="shared" si="8"/>
-        <v>333333333333333.31</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="5"/>
-        <v>333343333433333.69</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="6"/>
-        <v>10000100000.375</v>
-      </c>
-      <c r="G13" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="M13" s="7">
         <f t="shared" si="9"/>
-        <v>333333333.33333331</v>
-      </c>
-      <c r="H13" s="7">
-        <f t="shared" si="10"/>
-        <v>10000.100000375</v>
-      </c>
-      <c r="I13" s="3">
-        <f t="shared" si="11"/>
-        <v>566666666666.66663</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="12"/>
-        <v>17000170.000637498</v>
-      </c>
-      <c r="L13" s="6">
-        <f t="shared" si="7"/>
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- new bonding curve numbers - happy path gem tests - more tests around bonding curve
</commit_message>
<xml_diff>
--- a/solidity/deep-gems-numbers.xlsx
+++ b/solidity/deep-gems-numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jehan/projects/deepgems/solidity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4AD799-81D8-3C43-A4DC-45AADF8CB493}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E8702B-594C-BD41-97EE-D1D070968968}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{71828AD9-EA99-1C4A-A456-5EB5551B9F92}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>unscaled ..1</t>
   </si>
@@ -63,7 +63,13 @@
     <t>Dollar cost to mint one gem with 100 psi</t>
   </si>
   <si>
-    <t>Gem number (approx)</t>
+    <t>Mint one gem with 200 psi</t>
+  </si>
+  <si>
+    <t>Gem number 100 psi</t>
+  </si>
+  <si>
+    <t>Gem number 200 psi</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3F3CE4-B0B2-B443-B4D2-87B823B17513}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,17 +477,20 @@
     <col min="10" max="10" width="22.83203125" customWidth="1"/>
     <col min="11" max="11" width="34.6640625" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="21.83203125" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="5">
-        <v>1000000000000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2000000000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -489,7 +498,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -521,10 +530,16 @@
         <v>8</v>
       </c>
       <c r="M4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>100</v>
       </c>
@@ -543,23 +558,23 @@
       </c>
       <c r="G5" s="8">
         <f t="shared" ref="G5:G6" si="1">C5/$B$1</f>
-        <v>3.333333333333333E-7</v>
+        <v>1.6666666666666665E-7</v>
       </c>
       <c r="H5" s="8">
         <f>E5/$B$1</f>
-        <v>1.0100333333333372E-8</v>
+        <v>5.0501666666666859E-9</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" ref="I5:I6" si="2">G5*$B$2</f>
-        <v>5.666666666666666E-4</v>
+        <v>2.833333333333333E-4</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:J6" si="3">H5*$B$2</f>
-        <v>1.7170566666666732E-5</v>
+        <v>8.5852833333333661E-6</v>
       </c>
       <c r="K5" s="3">
         <f>J5*100</f>
-        <v>1.7170566666666733E-3</v>
+        <v>8.5852833333333663E-4</v>
       </c>
       <c r="L5" s="6">
         <f>A5</f>
@@ -569,8 +584,16 @@
         <f>L5/100</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="3">
+        <f>K5*2</f>
+        <v>1.7170566666666733E-3</v>
+      </c>
+      <c r="O5" s="3">
+        <f>M5/2</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1000</v>
       </c>
@@ -589,34 +612,42 @@
       </c>
       <c r="G6" s="8">
         <f t="shared" si="1"/>
-        <v>3.3333333333333332E-4</v>
+        <v>1.6666666666666666E-4</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" ref="H5:H6" si="6">E6/$B$1</f>
-        <v>1.001000333333373E-6</v>
+        <f t="shared" ref="H6" si="6">E6/$B$1</f>
+        <v>5.0050016666668649E-7</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" si="2"/>
-        <v>0.56666666666666665</v>
+        <v>0.28333333333333333</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="3"/>
-        <v>1.7017005666667342E-3</v>
+        <v>8.5085028333336708E-4</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" ref="K6:K13" si="7">J6*100</f>
+        <f>J6*100</f>
+        <v>8.5085028333336712E-2</v>
+      </c>
+      <c r="L6" s="6">
+        <f>A6</f>
+        <v>1000</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" ref="M6:M13" si="7">L6/100</f>
+        <v>10</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" ref="N6:N13" si="8">K6*2</f>
         <v>0.17017005666667342</v>
       </c>
-      <c r="L6" s="6">
-        <f t="shared" ref="L6:L13" si="8">A6</f>
-        <v>1000</v>
-      </c>
-      <c r="M6" s="7">
-        <f t="shared" ref="M6:M13" si="9">L6/100</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O6" s="3">
+        <f>M6/2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>10000</v>
       </c>
@@ -635,40 +666,48 @@
       </c>
       <c r="G7" s="8">
         <f>C7/$B$1</f>
-        <v>0.33333333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H7" s="8">
         <f>E7/$B$1</f>
-        <v>1.0001000033337402E-4</v>
+        <v>5.000500016668701E-5</v>
       </c>
       <c r="I7" s="3">
         <f>G7*$B$2</f>
-        <v>566.66666666666663</v>
+        <v>283.33333333333331</v>
       </c>
       <c r="J7" s="3">
         <f>H7*$B$2</f>
-        <v>0.17001700056673583</v>
+        <v>8.5008500283367913E-2</v>
       </c>
       <c r="K7" s="3">
+        <f>J7*100</f>
+        <v>8.5008500283367905</v>
+      </c>
+      <c r="L7" s="6">
+        <f>A7</f>
+        <v>10000</v>
+      </c>
+      <c r="M7" s="7">
         <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="8"/>
         <v>17.001700056673581</v>
       </c>
-      <c r="L7" s="6">
-        <f t="shared" si="8"/>
-        <v>10000</v>
-      </c>
-      <c r="M7" s="7">
-        <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O7" s="3">
+        <f>M7/2</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>20000</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="2">
-        <f t="shared" ref="C8:C13" si="10">(A8^3 / 3)</f>
+        <f t="shared" ref="C8:C13" si="9">(A8^3 / 3)</f>
         <v>2666666666666.6665</v>
       </c>
       <c r="D8" s="3">
@@ -680,41 +719,49 @@
         <v>400020000.33349609</v>
       </c>
       <c r="G8" s="8">
-        <f t="shared" ref="G8:G13" si="11">C8/$B$1</f>
-        <v>2.6666666666666665</v>
+        <f t="shared" ref="G8:G13" si="10">C8/$B$1</f>
+        <v>1.3333333333333333</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" ref="H8:H13" si="12">E8/$B$1</f>
-        <v>4.000200003334961E-4</v>
+        <f t="shared" ref="H8:H13" si="11">E8/$B$1</f>
+        <v>2.0001000016674805E-4</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" ref="I8:I13" si="13">G8*$B$2</f>
-        <v>4533.333333333333</v>
+        <f t="shared" ref="I8:I13" si="12">G8*$B$2</f>
+        <v>2266.6666666666665</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" ref="J8:J13" si="14">H8*$B$2</f>
-        <v>0.68003400056694341</v>
+        <f t="shared" ref="J8:J13" si="13">H8*$B$2</f>
+        <v>0.3400170002834717</v>
       </c>
       <c r="K8" s="3">
+        <f>J8*100</f>
+        <v>34.001700028347173</v>
+      </c>
+      <c r="L8" s="6">
+        <f>A8</f>
+        <v>20000</v>
+      </c>
+      <c r="M8" s="7">
         <f t="shared" si="7"/>
+        <v>200</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="8"/>
         <v>68.003400056694346</v>
       </c>
-      <c r="L8" s="6">
-        <f t="shared" si="8"/>
-        <v>20000</v>
-      </c>
-      <c r="M8" s="7">
-        <f t="shared" si="9"/>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O8" s="3">
+        <f>M8/2</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>30000</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>9000000000000</v>
       </c>
       <c r="D9" s="3">
@@ -726,133 +773,157 @@
         <v>900030000.33398438</v>
       </c>
       <c r="G9" s="8">
+        <f t="shared" si="10"/>
+        <v>4.5</v>
+      </c>
+      <c r="H9" s="8">
         <f t="shared" si="11"/>
-        <v>9</v>
-      </c>
-      <c r="H9" s="8">
+        <v>4.5001500016699219E-4</v>
+      </c>
+      <c r="I9" s="3">
         <f t="shared" si="12"/>
-        <v>9.0003000033398437E-4</v>
-      </c>
-      <c r="I9" s="3">
+        <v>7650</v>
+      </c>
+      <c r="J9" s="3">
         <f t="shared" si="13"/>
-        <v>15300</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="14"/>
-        <v>1.5300510005677734</v>
+        <v>0.76502550028388672</v>
       </c>
       <c r="K9" s="3">
+        <f>J9*100</f>
+        <v>76.502550028388669</v>
+      </c>
+      <c r="L9" s="6">
+        <f>A9</f>
+        <v>30000</v>
+      </c>
+      <c r="M9" s="7">
         <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="8"/>
         <v>153.00510005677734</v>
       </c>
-      <c r="L9" s="6">
-        <f t="shared" si="8"/>
-        <v>30000</v>
-      </c>
-      <c r="M9" s="7">
-        <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O9" s="3">
+        <f>M9/2</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>200000</v>
+        <v>50000</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2">
-        <f t="shared" si="10"/>
-        <v>2666666666666666.5</v>
+        <f t="shared" si="9"/>
+        <v>41666666666666.664</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="4"/>
-        <v>2666706666866667</v>
+        <v>41669166716667</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="5"/>
-        <v>40000200000.5</v>
+        <v>2500050000.3359375</v>
       </c>
       <c r="G10" s="8">
+        <f t="shared" si="10"/>
+        <v>20.833333333333332</v>
+      </c>
+      <c r="H10" s="8">
         <f t="shared" si="11"/>
-        <v>2666.6666666666665</v>
-      </c>
-      <c r="H10" s="8">
+        <v>1.2500250001679688E-3</v>
+      </c>
+      <c r="I10" s="3">
         <f t="shared" si="12"/>
-        <v>4.0000200000500002E-2</v>
-      </c>
-      <c r="I10" s="3">
+        <v>35416.666666666664</v>
+      </c>
+      <c r="J10" s="3">
         <f t="shared" si="13"/>
-        <v>4533333.333333333</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="14"/>
-        <v>68.000340000850002</v>
+        <v>2.1250425002855469</v>
       </c>
       <c r="K10" s="3">
+        <f>J10*100</f>
+        <v>212.50425002855468</v>
+      </c>
+      <c r="L10" s="6">
+        <f>A10</f>
+        <v>50000</v>
+      </c>
+      <c r="M10" s="7">
         <f t="shared" si="7"/>
-        <v>6800.0340000850001</v>
-      </c>
-      <c r="L10" s="6">
+        <v>500</v>
+      </c>
+      <c r="N10" s="3">
         <f t="shared" si="8"/>
+        <v>425.00850005710936</v>
+      </c>
+      <c r="O10" s="3">
+        <f>M10/2</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>200000</v>
-      </c>
-      <c r="M10" s="7">
-        <f t="shared" si="9"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <v>900000</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2">
-        <f t="shared" si="10"/>
-        <v>2.43E+17</v>
+        <f t="shared" si="9"/>
+        <v>2666666666666666.5</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="4"/>
-        <v>2.430008100009E+17</v>
+        <v>2666706666866667</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="5"/>
-        <v>810000900000</v>
+        <v>40000200000.5</v>
       </c>
       <c r="G11" s="8">
+        <f t="shared" si="10"/>
+        <v>1333.3333333333333</v>
+      </c>
+      <c r="H11" s="8">
         <f t="shared" si="11"/>
-        <v>243000</v>
-      </c>
-      <c r="H11" s="8">
+        <v>2.0000100000250001E-2</v>
+      </c>
+      <c r="I11" s="3">
         <f t="shared" si="12"/>
-        <v>0.81000090000000002</v>
-      </c>
-      <c r="I11" s="3">
+        <v>2266666.6666666665</v>
+      </c>
+      <c r="J11" s="3">
         <f t="shared" si="13"/>
-        <v>413100000</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="14"/>
-        <v>1377.00153</v>
+        <v>34.000170000425001</v>
       </c>
       <c r="K11" s="3">
+        <f>J11*100</f>
+        <v>3400.0170000425001</v>
+      </c>
+      <c r="L11" s="6">
+        <f>A11</f>
+        <v>200000</v>
+      </c>
+      <c r="M11" s="7">
         <f t="shared" si="7"/>
-        <v>137700.15299999999</v>
-      </c>
-      <c r="L11" s="6">
+        <v>2000</v>
+      </c>
+      <c r="N11" s="3">
         <f t="shared" si="8"/>
-        <v>900000</v>
-      </c>
-      <c r="M11" s="7">
-        <f t="shared" si="9"/>
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>6800.0340000850001</v>
+      </c>
+      <c r="O11" s="3">
+        <f>M11/2</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>1000000</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>3.3333333333333331E+17</v>
       </c>
       <c r="D12" s="3">
@@ -864,78 +935,94 @@
         <v>1000001000064</v>
       </c>
       <c r="G12" s="8">
+        <f t="shared" si="10"/>
+        <v>166666.66666666666</v>
+      </c>
+      <c r="H12" s="8">
         <f t="shared" si="11"/>
-        <v>333333.33333333331</v>
-      </c>
-      <c r="H12" s="8">
+        <v>0.50000050003200003</v>
+      </c>
+      <c r="I12" s="3">
         <f t="shared" si="12"/>
-        <v>1.0000010000640001</v>
-      </c>
-      <c r="I12" s="3">
+        <v>283333333.33333331</v>
+      </c>
+      <c r="J12" s="3">
         <f t="shared" si="13"/>
-        <v>566666666.66666663</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="14"/>
-        <v>1700.0017001088002</v>
+        <v>850.00085005440008</v>
       </c>
       <c r="K12" s="3">
+        <f>J12*100</f>
+        <v>85000.085005440007</v>
+      </c>
+      <c r="L12" s="6">
+        <f>A12</f>
+        <v>1000000</v>
+      </c>
+      <c r="M12" s="7">
         <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="8"/>
         <v>170000.17001088001</v>
       </c>
-      <c r="L12" s="6">
-        <f t="shared" si="8"/>
-        <v>1000000</v>
-      </c>
-      <c r="M12" s="7">
-        <f t="shared" si="9"/>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O12" s="3">
+        <f>M12/2</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>10000000</v>
+        <v>2000000</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2">
-        <f t="shared" si="10"/>
-        <v>3.3333333333333331E+20</v>
+        <f t="shared" si="9"/>
+        <v>2.6666666666666665E+18</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="4"/>
-        <v>3.3333343333334332E+20</v>
+        <v>2.6666706666686664E+18</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="5"/>
-        <v>100000010010624</v>
+        <v>4000001999872</v>
       </c>
       <c r="G13" s="8">
+        <f t="shared" si="10"/>
+        <v>1333333.3333333333</v>
+      </c>
+      <c r="H13" s="8">
         <f t="shared" si="11"/>
-        <v>333333333.33333331</v>
-      </c>
-      <c r="H13" s="8">
+        <v>2.0000009999359998</v>
+      </c>
+      <c r="I13" s="3">
         <f t="shared" si="12"/>
-        <v>100.000010010624</v>
-      </c>
-      <c r="I13" s="3">
+        <v>2266666666.6666665</v>
+      </c>
+      <c r="J13" s="3">
         <f t="shared" si="13"/>
-        <v>566666666666.66663</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="14"/>
-        <v>170000.01701806078</v>
+        <v>3400.0016998911997</v>
       </c>
       <c r="K13" s="3">
+        <f>J13*100</f>
+        <v>340000.16998911998</v>
+      </c>
+      <c r="L13" s="6">
+        <f>A13</f>
+        <v>2000000</v>
+      </c>
+      <c r="M13" s="7">
         <f t="shared" si="7"/>
-        <v>17000001.70180608</v>
-      </c>
-      <c r="L13" s="6">
+        <v>20000</v>
+      </c>
+      <c r="N13" s="3">
         <f t="shared" si="8"/>
-        <v>10000000</v>
-      </c>
-      <c r="M13" s="7">
-        <f t="shared" si="9"/>
-        <v>100000</v>
+        <v>680000.33997823996</v>
+      </c>
+      <c r="O13" s="3">
+        <f>M13/2</f>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>